<commit_message>
+ j column for favourite time in statements
</commit_message>
<xml_diff>
--- a/data/ЕКОНОМІЧНОЇ ТЕОРІЇ ТА ПІДПРИЄМНИЦТВА_ВІДОМІСТЬ ДОРУЧЕНЬ - 2020.xlsx
+++ b/data/ЕКОНОМІЧНОЇ ТЕОРІЇ ТА ПІДПРИЄМНИЦТВА_ВІДОМІСТЬ ДОРУЧЕНЬ - 2020.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$I$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Лист1!$A$1:$J$81</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="95">
   <si>
     <t>МІНІСТЕРСТВО ОСВІТИ І НАУКИ УКРАЇНИ</t>
   </si>
@@ -118,10 +118,6 @@
     <t>Мікроекономіка</t>
   </si>
   <si>
-    <t>Кригульська Тетяна 
-Борисівна</t>
-  </si>
-  <si>
     <t>Губарь Олена Василівна</t>
   </si>
   <si>
@@ -351,6 +347,9 @@
   </si>
   <si>
     <t>Федорченко Ольга Костянтинівна</t>
+  </si>
+  <si>
+    <t>Кригульська Тетяна Борисівна</t>
   </si>
 </sst>
 </file>
@@ -454,12 +453,18 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -490,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -538,6 +543,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -557,6 +568,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -843,10 +863,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M81"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="D62" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,48 +877,50 @@
     <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
     <col min="5" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="8" max="9" width="24.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I1" s="13" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="N1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="3" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.4">
-      <c r="A4" s="19" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.4">
+      <c r="A4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:13" ht="6.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" spans="1:14" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -908,21 +930,23 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:13" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" spans="1:14" ht="8.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -931,22 +955,24 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="I7" s="17"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-    </row>
-    <row r="9" spans="1:13" ht="11.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" ht="11.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -955,35 +981,38 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -992,9 +1021,10 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="18"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1022,8 +1052,11 @@
       <c r="I13" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J13" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>1</v>
       </c>
@@ -1051,8 +1084,11 @@
       <c r="I14" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>1</v>
       </c>
@@ -1060,7 +1096,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>19</v>
@@ -1072,16 +1108,17 @@
         <v>2</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J15" s="28"/>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>2</v>
       </c>
@@ -1089,10 +1126,10 @@
         <v>20</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="15">
         <v>30</v>
@@ -1101,16 +1138,17 @@
         <v>2</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J16" s="28"/>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>3</v>
       </c>
@@ -1118,7 +1156,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>19</v>
@@ -1130,16 +1168,17 @@
         <v>2</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J17" s="28"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>4</v>
       </c>
@@ -1147,10 +1186,10 @@
         <v>21</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="15">
         <v>14</v>
@@ -1159,16 +1198,17 @@
         <v>1</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J18" s="28"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>5</v>
       </c>
@@ -1176,10 +1216,10 @@
         <v>21</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="15">
         <v>14</v>
@@ -1188,16 +1228,17 @@
         <v>1</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J19" s="28"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>6</v>
       </c>
@@ -1205,7 +1246,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>19</v>
@@ -1217,16 +1258,17 @@
         <v>2</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J20" s="28"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>7</v>
       </c>
@@ -1234,10 +1276,10 @@
         <v>21</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="15">
         <v>30</v>
@@ -1246,16 +1288,17 @@
         <v>2</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>8</v>
       </c>
@@ -1263,10 +1306,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="15">
         <v>30</v>
@@ -1275,16 +1318,17 @@
         <v>2</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J22" s="28"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>9</v>
       </c>
@@ -1292,7 +1336,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>19</v>
@@ -1304,16 +1348,17 @@
         <v>2</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J23" s="28"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>10</v>
       </c>
@@ -1321,10 +1366,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E24" s="15">
         <v>30</v>
@@ -1333,24 +1378,25 @@
         <v>2</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J24" s="28"/>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>11</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>19</v>
@@ -1362,27 +1408,28 @@
         <v>2</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J25" s="28"/>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>12</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="15">
         <v>14</v>
@@ -1391,53 +1438,55 @@
         <v>1</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J26" s="28"/>
+    </row>
+    <row r="27" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>13</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="15">
+        <v>14</v>
+      </c>
+      <c r="F27" s="15">
+        <v>1</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="28"/>
+    </row>
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>14</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>42</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="15">
-        <v>14</v>
-      </c>
-      <c r="F27" s="15">
-        <v>1</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
-        <v>14</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>19</v>
@@ -1449,16 +1498,17 @@
         <v>2</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J28" s="28"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>15</v>
       </c>
@@ -1466,10 +1516,10 @@
         <v>18</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" s="15">
         <v>14</v>
@@ -1478,16 +1528,17 @@
         <v>1</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J29" s="28"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>16</v>
       </c>
@@ -1495,10 +1546,10 @@
         <v>18</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" s="15">
         <v>14</v>
@@ -1507,16 +1558,17 @@
         <v>1</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J30" s="28"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>17</v>
       </c>
@@ -1524,36 +1576,37 @@
         <v>18</v>
       </c>
       <c r="C31" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="15">
+        <v>14</v>
+      </c>
+      <c r="F31" s="15">
+        <v>1</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J31" s="28"/>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>18</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>46</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="15">
-        <v>14</v>
-      </c>
-      <c r="F31" s="15">
-        <v>1</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
-        <v>18</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>19</v>
@@ -1565,16 +1618,17 @@
         <v>1</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J32" s="28"/>
+    </row>
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>19</v>
       </c>
@@ -1582,10 +1636,10 @@
         <v>18</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" s="15">
         <v>14</v>
@@ -1594,16 +1648,17 @@
         <v>1</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J33" s="28"/>
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>20</v>
       </c>
@@ -1611,7 +1666,7 @@
         <v>18</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>19</v>
@@ -1623,16 +1678,17 @@
         <v>1</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J34" s="28"/>
+    </row>
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>21</v>
       </c>
@@ -1640,10 +1696,10 @@
         <v>18</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="15">
         <v>14</v>
@@ -1652,16 +1708,17 @@
         <v>1</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J35" s="28"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>22</v>
       </c>
@@ -1669,10 +1726,10 @@
         <v>18</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" s="15">
         <v>14</v>
@@ -1681,16 +1738,17 @@
         <v>1</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J36" s="28"/>
+    </row>
+    <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>23</v>
       </c>
@@ -1698,7 +1756,7 @@
         <v>18</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>19</v>
@@ -1710,16 +1768,17 @@
         <v>1</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J37" s="28"/>
+    </row>
+    <row r="38" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>24</v>
       </c>
@@ -1727,10 +1786,10 @@
         <v>18</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38" s="15">
         <v>14</v>
@@ -1739,16 +1798,17 @@
         <v>1</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>25</v>
       </c>
@@ -1756,36 +1816,37 @@
         <v>18</v>
       </c>
       <c r="C39" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="15">
+        <v>14</v>
+      </c>
+      <c r="F39" s="15">
+        <v>1</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>26</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="16" t="s">
         <v>53</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" s="15">
-        <v>14</v>
-      </c>
-      <c r="F39" s="15">
-        <v>1</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
-        <v>26</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>54</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>19</v>
@@ -1797,16 +1858,17 @@
         <v>1</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J40" s="28"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>27</v>
       </c>
@@ -1814,10 +1876,10 @@
         <v>18</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E41" s="15">
         <v>14</v>
@@ -1826,16 +1888,17 @@
         <v>1</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J41" s="28"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>28</v>
       </c>
@@ -1843,68 +1906,70 @@
         <v>18</v>
       </c>
       <c r="C42" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="15">
+        <v>14</v>
+      </c>
+      <c r="F42" s="15">
+        <v>1</v>
+      </c>
+      <c r="G42" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J42" s="28"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>29</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" s="15">
-        <v>14</v>
-      </c>
-      <c r="F42" s="15">
-        <v>1</v>
-      </c>
-      <c r="G42" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I42" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
-        <v>29</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="14" t="s">
+      <c r="D43" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="15">
+        <v>14</v>
+      </c>
+      <c r="F43" s="15">
+        <v>1</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J43" s="28"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>30</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="15">
-        <v>14</v>
-      </c>
-      <c r="F43" s="15">
-        <v>1</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I43" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
-        <v>30</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="D44" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" s="15">
         <v>14</v>
@@ -1913,16 +1978,17 @@
         <v>1</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J44" s="28"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>31</v>
       </c>
@@ -1930,7 +1996,7 @@
         <v>18</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>19</v>
@@ -1942,16 +2008,17 @@
         <v>1</v>
       </c>
       <c r="G45" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H45" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H45" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="I45" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J45" s="28"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>32</v>
       </c>
@@ -1959,10 +2026,10 @@
         <v>18</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E46" s="15">
         <v>14</v>
@@ -1971,16 +2038,17 @@
         <v>1</v>
       </c>
       <c r="G46" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H46" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="I46" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J46" s="28"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>33</v>
       </c>
@@ -1988,7 +2056,7 @@
         <v>18</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47" s="15" t="s">
         <v>19</v>
@@ -2000,16 +2068,17 @@
         <v>1</v>
       </c>
       <c r="G47" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H47" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H47" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="I47" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J47" s="28"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>34</v>
       </c>
@@ -2017,10 +2086,10 @@
         <v>18</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48" s="15">
         <v>14</v>
@@ -2029,16 +2098,17 @@
         <v>1</v>
       </c>
       <c r="G48" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H48" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H48" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="I48" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J48" s="28"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>35</v>
       </c>
@@ -2046,10 +2116,10 @@
         <v>18</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49" s="15">
         <v>14</v>
@@ -2058,16 +2128,17 @@
         <v>1</v>
       </c>
       <c r="G49" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H49" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="I49" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J49" s="28"/>
+    </row>
+    <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>36</v>
       </c>
@@ -2075,7 +2146,7 @@
         <v>18</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>19</v>
@@ -2087,16 +2158,17 @@
         <v>1</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J50" s="28"/>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>37</v>
       </c>
@@ -2104,10 +2176,10 @@
         <v>18</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" s="15">
         <v>14</v>
@@ -2116,16 +2188,17 @@
         <v>1</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H51" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J51" s="28"/>
+    </row>
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>38</v>
       </c>
@@ -2133,10 +2206,10 @@
         <v>18</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E52" s="15">
         <v>14</v>
@@ -2145,16 +2218,17 @@
         <v>1</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J52" s="28"/>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>39</v>
       </c>
@@ -2162,7 +2236,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>19</v>
@@ -2174,16 +2248,17 @@
         <v>1</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H53" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J53" s="28"/>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>40</v>
       </c>
@@ -2191,10 +2266,10 @@
         <v>18</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E54" s="15">
         <v>14</v>
@@ -2203,16 +2278,17 @@
         <v>1</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H54" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J54" s="28"/>
+    </row>
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>41</v>
       </c>
@@ -2220,10 +2296,10 @@
         <v>18</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E55" s="15">
         <v>14</v>
@@ -2232,16 +2308,17 @@
         <v>1</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J55" s="28"/>
+    </row>
+    <row r="56" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>42</v>
       </c>
@@ -2249,7 +2326,7 @@
         <v>18</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>19</v>
@@ -2261,16 +2338,17 @@
         <v>1</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H56" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J56" s="28"/>
+    </row>
+    <row r="57" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>43</v>
       </c>
@@ -2278,10 +2356,10 @@
         <v>18</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E57" s="15">
         <v>14</v>
@@ -2290,16 +2368,17 @@
         <v>1</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J57" s="28"/>
+    </row>
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>44</v>
       </c>
@@ -2307,10 +2386,10 @@
         <v>18</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E58" s="15">
         <v>14</v>
@@ -2319,16 +2398,17 @@
         <v>1</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J58" s="28"/>
+    </row>
+    <row r="59" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>45</v>
       </c>
@@ -2336,7 +2416,7 @@
         <v>18</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>19</v>
@@ -2348,16 +2428,17 @@
         <v>1</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J59" s="28"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>46</v>
       </c>
@@ -2365,10 +2446,10 @@
         <v>18</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E60" s="15">
         <v>14</v>
@@ -2377,16 +2458,17 @@
         <v>1</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J60" s="28"/>
+    </row>
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>47</v>
       </c>
@@ -2394,10 +2476,10 @@
         <v>18</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E61" s="15">
         <v>14</v>
@@ -2406,16 +2488,17 @@
         <v>1</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J61" s="28"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>48</v>
       </c>
@@ -2423,10 +2506,10 @@
         <v>18</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E62" s="15">
         <v>14</v>
@@ -2435,16 +2518,17 @@
         <v>1</v>
       </c>
       <c r="G62" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J62" s="28"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>49</v>
       </c>
@@ -2452,10 +2536,10 @@
         <v>18</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E63" s="15">
         <v>14</v>
@@ -2464,16 +2548,17 @@
         <v>1</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J63" s="28"/>
+    </row>
+    <row r="64" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>50</v>
       </c>
@@ -2481,7 +2566,7 @@
         <v>18</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D64" s="15" t="s">
         <v>19</v>
@@ -2493,16 +2578,17 @@
         <v>1</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H64" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J64" s="28"/>
+    </row>
+    <row r="65" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>51</v>
       </c>
@@ -2510,10 +2596,10 @@
         <v>18</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E65" s="15">
         <v>14</v>
@@ -2522,16 +2608,17 @@
         <v>1</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H65" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J65" s="28"/>
+    </row>
+    <row r="66" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <v>52</v>
       </c>
@@ -2539,10 +2626,10 @@
         <v>18</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D66" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E66" s="15">
         <v>14</v>
@@ -2551,16 +2638,17 @@
         <v>1</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H66" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J66" s="28"/>
+    </row>
+    <row r="67" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>52</v>
       </c>
@@ -2568,10 +2656,10 @@
         <v>18</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E67" s="15">
         <v>14</v>
@@ -2580,16 +2668,17 @@
         <v>1</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J67" s="28"/>
+    </row>
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>53</v>
       </c>
@@ -2597,7 +2686,7 @@
         <v>18</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" s="15" t="s">
         <v>19</v>
@@ -2609,16 +2698,17 @@
         <v>1</v>
       </c>
       <c r="G68" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I68" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J68" s="28"/>
+    </row>
+    <row r="69" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>55</v>
       </c>
@@ -2626,10 +2716,10 @@
         <v>18</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E69" s="15">
         <v>14</v>
@@ -2638,16 +2728,17 @@
         <v>1</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I69" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J69" s="28"/>
+    </row>
+    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <v>56</v>
       </c>
@@ -2655,10 +2746,10 @@
         <v>18</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E70" s="15">
         <v>14</v>
@@ -2667,16 +2758,17 @@
         <v>1</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I70" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J70" s="28"/>
+    </row>
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>57</v>
       </c>
@@ -2684,10 +2776,10 @@
         <v>18</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E71" s="15">
         <v>14</v>
@@ -2696,16 +2788,17 @@
         <v>1</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H71" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J71" s="28"/>
+    </row>
+    <row r="72" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>58</v>
       </c>
@@ -2713,7 +2806,7 @@
         <v>18</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D72" s="15" t="s">
         <v>19</v>
@@ -2725,16 +2818,17 @@
         <v>1</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H72" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I72" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J72" s="28"/>
+    </row>
+    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>59</v>
       </c>
@@ -2742,10 +2836,10 @@
         <v>18</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E73" s="15">
         <v>14</v>
@@ -2754,16 +2848,17 @@
         <v>1</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H73" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I73" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J73" s="28"/>
+    </row>
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <v>60</v>
       </c>
@@ -2771,10 +2866,10 @@
         <v>18</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E74" s="15">
         <v>14</v>
@@ -2783,16 +2878,17 @@
         <v>1</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H74" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I74" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J74" s="28"/>
+    </row>
+    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>61</v>
       </c>
@@ -2800,10 +2896,10 @@
         <v>18</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E75" s="15">
         <v>14</v>
@@ -2812,16 +2908,17 @@
         <v>1</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I75" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J75" s="28"/>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>62</v>
       </c>
@@ -2829,10 +2926,10 @@
         <v>18</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E76" s="15">
         <v>14</v>
@@ -2841,16 +2938,17 @@
         <v>1</v>
       </c>
       <c r="G76" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H76" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I76" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J76" s="28"/>
+    </row>
+    <row r="77" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>63</v>
       </c>
@@ -2858,7 +2956,7 @@
         <v>18</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>19</v>
@@ -2870,16 +2968,17 @@
         <v>1</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H77" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I77" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J77" s="28"/>
+    </row>
+    <row r="78" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <v>64</v>
       </c>
@@ -2887,10 +2986,10 @@
         <v>18</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E78" s="15">
         <v>14</v>
@@ -2899,16 +2998,17 @@
         <v>1</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H78" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I78" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="J78" s="28"/>
+    </row>
+    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>65</v>
       </c>
@@ -2916,10 +3016,10 @@
         <v>18</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E79" s="15">
         <v>14</v>
@@ -2928,53 +3028,56 @@
         <v>1</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H79" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" s="28"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="17"/>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
+      <c r="B80" s="19"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="17"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A81:I81"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="A80:J80"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="29" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="28" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>